<commit_message>
Update RSA data benchmark
</commit_message>
<xml_diff>
--- a/16KB.xlsx
+++ b/16KB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\Honours Project\Script\Data\16 KB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\Honours Project\Encryption algorithms performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A5EB88-7F4B-4DCD-945F-6D7D7D0ED9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593E6A1F-E48D-4B04-985B-ABA2C81C45D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="1365" windowWidth="16515" windowHeight="11745" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5610" yWindow="2805" windowWidth="16515" windowHeight="11745" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Difference" sheetId="2" r:id="rId1"/>
@@ -210,8 +210,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.0000"/>
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
@@ -372,38 +371,38 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -992,7 +991,7 @@
   <dimension ref="B3:I25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,7 +1032,7 @@
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="22" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1056,12 +1055,12 @@
       <c r="H4" s="12">
         <v>16</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="22" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="15"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1082,10 +1081,10 @@
       <c r="H5" s="12">
         <v>16</v>
       </c>
-      <c r="I5" s="15"/>
+      <c r="I5" s="22"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="15"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
@@ -1106,10 +1105,10 @@
       <c r="H6" s="12">
         <v>16</v>
       </c>
-      <c r="I6" s="15"/>
+      <c r="I6" s="22"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="15"/>
+      <c r="B7" s="22"/>
       <c r="C7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1130,10 +1129,10 @@
       <c r="H7" s="12">
         <v>16</v>
       </c>
-      <c r="I7" s="15"/>
+      <c r="I7" s="22"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="15"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="3" t="s">
         <v>2</v>
       </c>
@@ -1154,10 +1153,10 @@
       <c r="H8" s="12">
         <v>16</v>
       </c>
-      <c r="I8" s="15"/>
+      <c r="I8" s="22"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="22" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1180,10 +1179,10 @@
       <c r="H9" s="12">
         <v>16</v>
       </c>
-      <c r="I9" s="15"/>
+      <c r="I9" s="22"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
@@ -1204,10 +1203,10 @@
       <c r="H10" s="12">
         <v>16</v>
       </c>
-      <c r="I10" s="15"/>
+      <c r="I10" s="22"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="15"/>
+      <c r="B11" s="22"/>
       <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
@@ -1228,27 +1227,27 @@
       <c r="H11" s="12">
         <v>16</v>
       </c>
-      <c r="I11" s="15"/>
+      <c r="I11" s="22"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="15"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="23">
-        <v>2.163E-2</v>
-      </c>
-      <c r="E12" s="24">
-        <v>1.44452</v>
-      </c>
-      <c r="F12" s="23">
-        <v>0.92930999999999997</v>
-      </c>
-      <c r="G12" s="24">
-        <v>3.36271E-2</v>
+      <c r="D12" s="24">
+        <v>1.1386E-2</v>
+      </c>
+      <c r="E12" s="25">
+        <v>1.3724000000000001</v>
+      </c>
+      <c r="F12" s="24">
+        <v>0.46404699999999999</v>
+      </c>
+      <c r="G12" s="25">
+        <v>3.3700000000000001E-2</v>
       </c>
       <c r="H12" s="12">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>31</v>
@@ -1271,7 +1270,7 @@
       <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="22"/>
+      <c r="B17" s="17"/>
       <c r="C17" s="9">
         <v>0.247449</v>
       </c>
@@ -1287,7 +1286,7 @@
       <c r="G17" s="9"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="22"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="9">
         <v>0.100355</v>
       </c>
@@ -1303,7 +1302,7 @@
       <c r="G18" s="9"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="22"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="9">
         <v>8.1149280000000008</v>
       </c>
@@ -1319,7 +1318,7 @@
       <c r="G19" s="9"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="22"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="9">
         <v>0.48256199999999999</v>
       </c>
@@ -1335,7 +1334,7 @@
       <c r="G20" s="9"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="22"/>
+      <c r="B21" s="17"/>
       <c r="C21" s="9">
         <v>0.48173199999999999</v>
       </c>
@@ -1351,7 +1350,7 @@
       <c r="G21" s="9"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="22"/>
+      <c r="B22" s="17"/>
       <c r="C22" s="9">
         <v>0.191279</v>
       </c>
@@ -1367,7 +1366,7 @@
       <c r="G22" s="9"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="22"/>
+      <c r="B23" s="17"/>
       <c r="C23" s="9">
         <v>0.24732499999999999</v>
       </c>
@@ -1383,7 +1382,7 @@
       <c r="G23" s="9"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="22"/>
+      <c r="B24" s="17"/>
       <c r="C24" s="9">
         <v>1.05616</v>
       </c>
@@ -1420,7 +1419,7 @@
   <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,12 +1446,12 @@
       <c r="E5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="22" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1461,80 +1460,80 @@
       <c r="D6" s="1">
         <v>16</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="16">
         <v>139296</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="16">
         <f>E6-3*D6*1024</f>
         <v>90144</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="15"/>
+      <c r="B7" s="22"/>
       <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="1">
         <v>16</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="16">
         <v>138720</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="16">
         <f t="shared" ref="F7:F13" si="0">E7-3*D7*1024</f>
         <v>89568</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="15"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="1">
         <v>16</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="16">
         <v>122944</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="16">
         <f t="shared" si="0"/>
         <v>73792</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="15"/>
+      <c r="B9" s="22"/>
       <c r="C9" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="1">
         <v>16</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="16">
         <v>138112</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="16">
         <f t="shared" si="0"/>
         <v>88960</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="1">
         <v>16</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="16">
         <v>138112</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="16">
         <f t="shared" si="0"/>
         <v>88960</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="22" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1543,60 +1542,59 @@
       <c r="D11" s="1">
         <v>16</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="16">
         <v>138480</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="16">
         <f t="shared" si="0"/>
         <v>89328</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="15"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="1">
         <v>16</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="16">
         <v>138112</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="16">
         <f t="shared" si="0"/>
         <v>88960</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="15"/>
+      <c r="B13" s="22"/>
       <c r="C13" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="1">
         <v>16</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="16">
         <v>138128</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="16">
         <f t="shared" si="0"/>
         <v>88976</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="15"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="1">
-        <v>32</v>
-      </c>
-      <c r="E14" s="18">
-        <v>196232</v>
-      </c>
-      <c r="F14" s="18">
-        <f>E14-D14*1024</f>
-        <v>163464</v>
+        <v>16</v>
+      </c>
+      <c r="E14" s="16">
+        <v>149432</v>
+      </c>
+      <c r="F14" s="16">
+        <v>149432</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1617,7 +1615,7 @@
   <dimension ref="A4:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1637,88 +1635,88 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="18">
         <v>3.7331300000000001E-4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="18">
         <v>1.9879199999999999E-4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="18">
         <v>1.1882916E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="18">
         <v>6.9143799999999995E-4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="25">
+      <c r="C9" s="18">
         <v>6.98224E-4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="23" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="18">
         <v>3.4650000000000002E-4</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="25">
+      <c r="C11" s="18">
         <v>3.80477E-4</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="18">
         <v>1.535472E-3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="14">
-        <v>0.85982800000000004</v>
+        <v>0.53676000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>